<commit_message>
update the xlsx files for connectivity example data
</commit_message>
<xml_diff>
--- a/braph2genesis/pipelines/connectivity/example data CON (DTI)/xls/GroupName2/covariates/GroupName2_covariates.xlsx
+++ b/braph2genesis/pipelines/connectivity/example data CON (DTI)/xls/GroupName2/covariates/GroupName2_covariates.xlsx
@@ -1,87 +1,254 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giovannivolpe/Documents/GitHub/Braph-2.0-Matlab/braph2genesis/pipelines/connectivity/example data CON (DTI)/xls/GroupName2/covariates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gunet-my.sharepoint.com/personal/yu-wei_chang_gu_se/Documents/ywc/projects/braph_example_data/Braph_ExampleData/Functional_ExampleData/GroupName2/covariates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A976530-C8BA-544C-9309-B76DAAFE0D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_714D654FCF63DA9DFE980FA4EE012D16618B0BCF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="14800" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2810" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
   <si>
+    <t>subject1</t>
+  </si>
+  <si>
+    <t>subject2</t>
+  </si>
+  <si>
+    <t>subject3</t>
+  </si>
+  <si>
+    <t>subject4</t>
+  </si>
+  <si>
+    <t>subject5</t>
+  </si>
+  <si>
+    <t>subject6</t>
+  </si>
+  <si>
+    <t>subject7</t>
+  </si>
+  <si>
+    <t>subject8</t>
+  </si>
+  <si>
+    <t>subject9</t>
+  </si>
+  <si>
+    <t>subject10</t>
+  </si>
+  <si>
+    <t>subject11</t>
+  </si>
+  <si>
+    <t>subject12</t>
+  </si>
+  <si>
+    <t>subject13</t>
+  </si>
+  <si>
+    <t>subject14</t>
+  </si>
+  <si>
+    <t>subject15</t>
+  </si>
+  <si>
+    <t>subject16</t>
+  </si>
+  <si>
+    <t>subject17</t>
+  </si>
+  <si>
+    <t>subject18</t>
+  </si>
+  <si>
+    <t>subject19</t>
+  </si>
+  <si>
+    <t>subject20</t>
+  </si>
+  <si>
+    <t>subject21</t>
+  </si>
+  <si>
+    <t>subject22</t>
+  </si>
+  <si>
+    <t>subject23</t>
+  </si>
+  <si>
+    <t>subject24</t>
+  </si>
+  <si>
+    <t>subject25</t>
+  </si>
+  <si>
+    <t>subject26</t>
+  </si>
+  <si>
+    <t>subject27</t>
+  </si>
+  <si>
+    <t>subject28</t>
+  </si>
+  <si>
+    <t>subject29</t>
+  </si>
+  <si>
+    <t>subject30</t>
+  </si>
+  <si>
+    <t>subject31</t>
+  </si>
+  <si>
+    <t>subject32</t>
+  </si>
+  <si>
+    <t>subject33</t>
+  </si>
+  <si>
+    <t>subject34</t>
+  </si>
+  <si>
+    <t>subject35</t>
+  </si>
+  <si>
+    <t>subject36</t>
+  </si>
+  <si>
+    <t>subject37</t>
+  </si>
+  <si>
+    <t>subject38</t>
+  </si>
+  <si>
+    <t>subject39</t>
+  </si>
+  <si>
+    <t>subject40</t>
+  </si>
+  <si>
+    <t>subject41</t>
+  </si>
+  <si>
+    <t>subject42</t>
+  </si>
+  <si>
+    <t>subject43</t>
+  </si>
+  <si>
+    <t>subject44</t>
+  </si>
+  <si>
+    <t>subject45</t>
+  </si>
+  <si>
+    <t>subject46</t>
+  </si>
+  <si>
+    <t>subject47</t>
+  </si>
+  <si>
+    <t>subject48</t>
+  </si>
+  <si>
+    <t>subject49</t>
+  </si>
+  <si>
+    <t>subject50</t>
+  </si>
+  <si>
     <t>age</t>
   </si>
   <si>
     <t>sex</t>
   </si>
   <si>
-    <t>female</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>SubjectID1</t>
-  </si>
-  <si>
-    <t>SubjectID2</t>
-  </si>
-  <si>
-    <t>SubjectID3</t>
-  </si>
-  <si>
-    <t>SubjectID4</t>
-  </si>
-  <si>
-    <t>SubjectID5</t>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>edu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,23 +271,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -429,81 +587,730 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="9.08984375" customWidth="1"/>
+    <col min="2" max="2" width="4.08984375" customWidth="1"/>
+    <col min="3" max="3" width="7.1796875" customWidth="1"/>
+    <col min="4" max="4" width="4.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B2">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B3">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
-        <v>90</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B6">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B7">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>76</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>77</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>65</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>52</v>
+      </c>
+      <c r="C15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>80</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="D19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25">
         <v>7</v>
       </c>
-      <c r="B4" s="1">
-        <v>85</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>63</v>
+      </c>
+      <c r="C28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>69</v>
+      </c>
+      <c r="C29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>67</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>73</v>
+      </c>
+      <c r="C32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>65</v>
+      </c>
+      <c r="C33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>51</v>
+      </c>
+      <c r="C34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>65</v>
+      </c>
+      <c r="D35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>61</v>
+      </c>
+      <c r="C36" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>63</v>
+      </c>
+      <c r="C37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>75</v>
+      </c>
+      <c r="C38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>60</v>
+      </c>
+      <c r="C39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39">
         <v>8</v>
       </c>
-      <c r="B5" s="1">
-        <v>55</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>57</v>
+      </c>
+      <c r="C40" t="s">
+        <v>66</v>
+      </c>
+      <c r="D40">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>62</v>
+      </c>
+      <c r="C41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>76</v>
+      </c>
+      <c r="C42" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>74</v>
+      </c>
+      <c r="C43" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>62</v>
+      </c>
+      <c r="C44" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>75</v>
+      </c>
+      <c r="C45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>52</v>
+      </c>
+      <c r="C46" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>78</v>
+      </c>
+      <c r="C47" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47">
         <v>9</v>
       </c>
-      <c r="B6" s="1">
-        <v>75</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>62</v>
+      </c>
+      <c r="C48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>72</v>
+      </c>
+      <c r="C49" t="s">
+        <v>71</v>
+      </c>
+      <c r="D49">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>61</v>
+      </c>
+      <c r="C50" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>53</v>
+      </c>
+      <c r="C51" t="s">
+        <v>71</v>
+      </c>
+      <c r="D51">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>